<commit_message>
Freq output file has descriptive headers
</commit_message>
<xml_diff>
--- a/files/extraction_summary.xlsx
+++ b/files/extraction_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1133,6 +1133,94 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1934</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1661</v>
+      </c>
+      <c r="D17" t="n">
+        <v>4</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1633</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>36.96</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>31.75</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>31.21</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2025-08-20 23:15:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1934</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1661</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1633</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>36.96</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>31.75</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>31.21</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2025-08-20 23:15:38</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>